<commit_message>
added baseline temp plot for comparison
</commit_message>
<xml_diff>
--- a/PF7111/TFB_20250307_378_HAND.xlsx
+++ b/PF7111/TFB_20250307_378_HAND.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mars/Documents/TPS/tps_py_tools/PF7111/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337E6C4F-8C22-B844-B9BB-9EC3CA8E6A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29933FC-E3E2-0146-BFE7-3FF44C5CD5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9040" yWindow="1940" windowWidth="21600" windowHeight="11380" xr2:uid="{4E2A18EF-6B8C-4620-8A6A-01E0FD4453E2}"/>
+    <workbookView xWindow="8640" yWindow="1940" windowWidth="21600" windowHeight="11380" xr2:uid="{4E2A18EF-6B8C-4620-8A6A-01E0FD4453E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Tower Fly By Data" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -496,7 +496,7 @@
         <v>2.7</v>
       </c>
       <c r="D3" s="1">
-        <v>2254</v>
+        <v>2251</v>
       </c>
       <c r="E3" s="1">
         <v>8.7799999999999994</v>

</xml_diff>